<commit_message>
chore: change sheet names in conductor_diagnostic.
To increase input file readability and understanding, sheet names in file conductor_diagnostic.xlsx where changed as follows:
    * Space becomes Spatial_discretization;
    * Time become Time_evolution.
The correspondig sub-folders in Output and Figures changes name as well and coherently.
</commit_message>
<xml_diff>
--- a/source_code/Description_of_Components/input_file_template/template_conductor_diagnostic.xlsx
+++ b/source_code/Description_of_Components/input_file_template/template_conductor_diagnostic.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politoit-my.sharepoint.com/personal/daniele_placido_polito_it/Documents/SC2_38/Description_of_Components/new_input_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politoit-my.sharepoint.com/personal/daniele_placido_polito_it/Documents/OPENSC2/source_code/Description_of_Components/input_file_template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{0D969C7C-59B6-4D41-9C8A-C3C1D111D96F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EF1D89CC-F3FB-49E0-8D9C-9B98A61C2353}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{0D969C7C-59B6-4D41-9C8A-C3C1D111D96F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E67D873C-0314-40F4-BCB5-343BD177E846}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Space" sheetId="1" r:id="rId1"/>
-    <sheet name="Time" sheetId="2" r:id="rId2"/>
+    <sheet name="Spatial_distribution" sheetId="1" r:id="rId1"/>
+    <sheet name="Time_evolution" sheetId="2" r:id="rId2"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId3"/>
@@ -254,6 +254,32 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
+      <sheetName val="CONDUCTOR_files"/>
+      <sheetName val="CONDUCTOR_input"/>
+      <sheetName val="CONDUCTOR_COUPLING"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="A1" t="str">
+            <v>CONDUCTOR</v>
+          </cell>
+          <cell r="E1">
+            <v>1</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
       <sheetName val="TRANSIENT"/>
     </sheetNames>
     <sheetDataSet>
@@ -273,32 +299,6 @@
           </cell>
         </row>
       </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="CONDUCTOR_files"/>
-      <sheetName val="CONDUCTOR_input"/>
-      <sheetName val="CONDUCTOR_COUPLING"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="1">
-          <cell r="A1" t="str">
-            <v>CONDUCTOR</v>
-          </cell>
-          <cell r="E1">
-            <v>1</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -569,7 +569,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
@@ -588,7 +588,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="str">
-        <f>[2]CONDUCTOR_files!$A$1</f>
+        <f>[1]CONDUCTOR_files!$A$1</f>
         <v>CONDUCTOR</v>
       </c>
       <c r="B1" s="17">
@@ -598,7 +598,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="3"/>
       <c r="E1" s="11">
-        <f>[2]CONDUCTOR_files!E$1</f>
+        <f>[1]CONDUCTOR_files!E$1</f>
         <v>1</v>
       </c>
     </row>
@@ -614,19 +614,19 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="str">
-        <f>[1]TRANSIENT!A$2</f>
+        <f>[2]TRANSIENT!A$2</f>
         <v>Variable name</v>
       </c>
       <c r="B3" s="10" t="str">
-        <f>[1]TRANSIENT!B$2</f>
+        <f>[2]TRANSIENT!B$2</f>
         <v>Unit</v>
       </c>
       <c r="C3" s="10" t="str">
-        <f>[1]TRANSIENT!C$2</f>
+        <f>[2]TRANSIENT!C$2</f>
         <v>Variable type</v>
       </c>
       <c r="D3" s="10" t="str">
-        <f>[1]TRANSIENT!D$2</f>
+        <f>[2]TRANSIENT!D$2</f>
         <v>Note/comments</v>
       </c>
       <c r="E3" s="11" t="str">
@@ -832,11 +832,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{470E6858-601C-4654-9D3B-60211F710697}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -852,17 +852,17 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="str">
-        <f>Space!A1</f>
+        <f>Spatial_distribution!A1</f>
         <v>CONDUCTOR</v>
       </c>
       <c r="B1" s="11">
-        <f>Space!B1</f>
+        <f>Spatial_distribution!B1</f>
         <v>1</v>
       </c>
       <c r="C1" s="12"/>
       <c r="D1" s="12"/>
       <c r="E1" s="11">
-        <f>Space!E1</f>
+        <f>Spatial_distribution!E1</f>
         <v>1</v>
       </c>
     </row>
@@ -872,29 +872,29 @@
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
       <c r="E2" s="11">
-        <f>Space!E2</f>
+        <f>Spatial_distribution!E2</f>
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="str">
-        <f>Space!A3</f>
+        <f>Spatial_distribution!A3</f>
         <v>Variable name</v>
       </c>
       <c r="B3" s="9" t="str">
-        <f>Space!B3</f>
+        <f>Spatial_distribution!B3</f>
         <v>Unit</v>
       </c>
       <c r="C3" s="9" t="str">
-        <f>Space!C3</f>
+        <f>Spatial_distribution!C3</f>
         <v>Variable type</v>
       </c>
       <c r="D3" s="9" t="str">
-        <f>Space!D3</f>
+        <f>Spatial_distribution!D3</f>
         <v>Note/comments</v>
       </c>
       <c r="E3" s="11" t="str">
-        <f>Space!E3</f>
+        <f>Spatial_distribution!E3</f>
         <v>CONDUCTOR_1</v>
       </c>
     </row>

</xml_diff>